<commit_message>
chore: Modiicado arquivos de saída
</commit_message>
<xml_diff>
--- a/outputs/atrib_limpos/tela3_params_clean.xlsx
+++ b/outputs/atrib_limpos/tela3_params_clean.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/accol/Library/Mobile Documents/com~apple~CloudDocs/UNIVERSIDADES/UFF/PROJETOS/PETROBRAS/PETRO_ProtecAI/protecai_testes/outputs/atrib_limpos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4CD931-6131-E14B-A470-2782A45F0B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5140" yWindow="500" windowWidth="21460" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clean" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -442,8 +448,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,12 +466,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -495,24 +507,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -550,7 +571,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -584,6 +605,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -618,9 +640,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -793,14 +816,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -828,7 +858,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -839,7 +869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -856,7 +886,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -867,7 +897,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -878,7 +908,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -889,7 +919,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -900,24 +930,24 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.64</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -928,7 +958,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -945,7 +975,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -962,7 +992,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -979,7 +1009,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -996,7 +1026,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1013,24 +1043,24 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>5.5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1047,24 +1077,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>0.3</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1081,24 +1111,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>0.125</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1115,24 +1145,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +1179,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1166,24 +1196,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1230,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1211,7 +1241,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1222,7 +1252,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1239,7 +1269,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1250,7 +1280,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1261,7 +1291,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1302,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1289,7 +1319,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1306,7 +1336,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1323,7 +1353,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1340,7 +1370,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1357,7 +1387,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1374,7 +1404,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1391,7 +1421,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1408,7 +1438,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1425,7 +1455,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1442,7 +1472,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1459,7 +1489,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1476,7 +1506,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1487,7 +1517,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1504,7 +1534,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1521,7 +1551,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1538,7 +1568,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1555,7 +1585,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>

</xml_diff>